<commit_message>
Update Day4 LIST FUNCTION( D FUNCTIONS).xlsx
</commit_message>
<xml_diff>
--- a/Advanced Excel For Data Analytics/Day4 LIST FUNCTION( D FUNCTIONS).xlsx
+++ b/Advanced Excel For Data Analytics/Day4 LIST FUNCTION( D FUNCTIONS).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Excel-For-Data-Analysis\Advanced Excel For Data Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBD502A-D36B-4AEC-8BC0-84CEDB7DDE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8D42C6-00AC-44AA-824C-A07F97139849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3930342E-F190-4108-9AFE-C16A349584CC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3930342E-F190-4108-9AFE-C16A349584CC}"/>
   </bookViews>
   <sheets>
     <sheet name="LIST FUNCTIONS DATABASE FUNCTIO" sheetId="1" r:id="rId1"/>
@@ -205,8 +205,30 @@
 </connections>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="128">
   <si>
     <t xml:space="preserve">LIST FUNCTIONS OR DATABASE FUNCTION
 THESE ARE IMPORTANT </t>
@@ -588,6 +610,9 @@
   </si>
   <si>
     <t>Image Check</t>
+  </si>
+  <si>
+    <t>X Look up</t>
   </si>
 </sst>
 </file>
@@ -596,9 +621,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,12 +638,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -662,12 +681,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="24"/>
@@ -872,65 +885,63 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="5" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="4" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
@@ -941,15 +952,10 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+      <border outline="0">
+        <top style="thin">
           <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -960,10 +966,15 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1040,7 +1051,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0E62410-907F-43E3-AB54-656B1F6A8A9F}" name="Food_Data" displayName="Food_Data" ref="A3:D93" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2" headerRowCellStyle="60% - Accent6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0E62410-907F-43E3-AB54-656B1F6A8A9F}" name="Food_Data" displayName="Food_Data" ref="A3:D93" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0" headerRowCellStyle="60% - Accent6">
   <autoFilter ref="A3:D93" xr:uid="{FA9B42F0-4950-4A36-99B7-52572DAEFD67}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{08255FD0-2A0E-4844-B533-112C2AD746B7}" name="Year"/>
@@ -1423,10 +1434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9B42F0-4950-4A36-99B7-52572DAEFD67}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D93"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1435,89 +1446,109 @@
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="8" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="F1" s="6" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="F1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="K2" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="K3" cm="1">
+        <f t="array" ref="K3:N3">_xlfn.XLOOKUP(H6,Food_Data[Food Name],Food_Data[],"Sorry",0,1)</f>
+        <v>2020</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Burger</v>
+      </c>
+      <c r="M3" t="str">
+        <v>Los Angeles</v>
+      </c>
+      <c r="N3">
+        <v>19430</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>2019</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="4">
         <v>23450</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>2020</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="4">
         <v>19430</v>
       </c>
-      <c r="F5" s="10">
-        <v>2019</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="3">
+        <v>2018</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2018</v>
       </c>
@@ -1530,31 +1561,31 @@
       <c r="D6">
         <v>30020</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="3">
         <v>2018</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>2021</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="4">
         <v>43200</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2022</v>
       </c>
@@ -1567,12 +1598,12 @@
       <c r="D8">
         <v>52300</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -1585,16 +1616,16 @@
       <c r="D9">
         <v>23800</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9">
+      <c r="G9" s="10"/>
+      <c r="H9" s="2">
         <f>DSUM(A3:D93,D3,F4:H6)</f>
-        <v>55500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>32050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -1607,38 +1638,38 @@
       <c r="D10">
         <v>19800</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9">
+      <c r="G10" s="10"/>
+      <c r="H10" s="2">
         <f>DMAX(A3:D93,D3,F4:H6)</f>
         <v>32050</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>2018</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="4">
         <v>32050</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9">
+      <c r="G11" s="10"/>
+      <c r="H11" s="2">
         <f>DMIN(A3:D93,D3,F4:H6)</f>
-        <v>23450</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>32050</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -1651,16 +1682,16 @@
       <c r="D12">
         <v>44200</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9">
+      <c r="G12" s="10"/>
+      <c r="H12" s="2">
         <f>DAVERAGE(A3:D93,D3,F4:H6)</f>
-        <v>27750</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>32050</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2022</v>
       </c>
@@ -1673,16 +1704,16 @@
       <c r="D13">
         <v>53450</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="12">
+      <c r="G13" s="10"/>
+      <c r="H13" s="5">
         <f>DCOUNT(A3:D93,D3,F4:H6)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2019</v>
       </c>
@@ -1696,7 +1727,7 @@
         <v>24800</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -1710,7 +1741,7 @@
         <v>20850</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1723,18 +1754,18 @@
       <c r="D16">
         <v>31520</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="15">
+      <c r="G16" s="10"/>
+      <c r="H16" s="7">
         <f>DSUM(Food_Data[#All],Food_Data[[#Headers],[Sales]],F4:H6)</f>
-        <v>55500</v>
-      </c>
-      <c r="J16" s="3" t="s">
+        <v>32050</v>
+      </c>
+      <c r="J16" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1749,11 +1780,11 @@
       <c r="D17">
         <v>45200</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="15">
+      <c r="G17" s="10"/>
+      <c r="H17" s="7">
         <f>DMAX(Food_Data[#All],Food_Data[[#Headers],[Sales]],F4:H6)</f>
         <v>32050</v>
       </c>
@@ -1771,13 +1802,13 @@
       <c r="D18">
         <v>51400</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="15">
+      <c r="G18" s="10"/>
+      <c r="H18" s="7">
         <f>DMIN(Food_Data[#All],Food_Data[[#Headers],[Sales]],F4:H6)</f>
-        <v>23450</v>
+        <v>32050</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1793,13 +1824,13 @@
       <c r="D19">
         <v>21800</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="15">
+      <c r="G19" s="10"/>
+      <c r="H19" s="7">
         <f>DAVERAGE(Food_Data[#All],Food_Data[[#Headers],[Sales]],F4:H6)</f>
-        <v>27750</v>
+        <v>32050</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1815,13 +1846,13 @@
       <c r="D20">
         <v>22030</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="15">
+      <c r="G20" s="10"/>
+      <c r="H20" s="7">
         <f>DCOUNT(Food_Data[#All],Food_Data[[#Headers],[Sales]],F4:H6)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1851,13 +1882,13 @@
       <c r="D22">
         <v>46500</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22">
+      <c r="G22" s="10"/>
+      <c r="H22" t="e">
         <f>DGET(Food_Data[#All], "Sales",F4:H5)</f>
-        <v>23450</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2855,22 +2886,23 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:I2"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F1:I2"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2884,7 +2916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0649BCA9-ABE2-4F8D-80C9-85D921FDCBDF}">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
@@ -2897,16 +2929,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2975,10 +3007,10 @@
       <c r="D5">
         <v>30020</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -3204,1149 +3236,1144 @@
       </c>
     </row>
     <row r="22" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A22" s="24">
+      <c r="A22">
         <v>2022</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22">
         <v>52300</v>
       </c>
     </row>
     <row r="23" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A23" s="24">
+      <c r="A23">
         <v>2019</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23">
         <v>25000</v>
       </c>
     </row>
     <row r="24" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A24" s="24">
+      <c r="A24">
         <v>2021</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24">
         <v>31500</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A25" s="24">
+      <c r="A25">
         <v>2020</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25">
         <v>19800</v>
       </c>
     </row>
     <row r="26" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A26" s="24">
+      <c r="A26">
         <v>2019</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26">
         <v>33000</v>
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A27" s="24">
+      <c r="A27">
         <v>2022</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27">
         <v>25500</v>
       </c>
     </row>
     <row r="28" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A28" s="24">
+      <c r="A28">
         <v>2020</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28">
         <v>19430</v>
       </c>
     </row>
     <row r="29" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A29" s="24">
+      <c r="A29">
         <v>2021</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29">
         <v>25300</v>
       </c>
     </row>
     <row r="30" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A30" s="24">
+      <c r="A30">
         <v>2020</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30">
         <v>24500</v>
       </c>
     </row>
     <row r="31" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A31" s="24">
+      <c r="A31">
         <v>2019</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31">
         <v>23800</v>
       </c>
     </row>
     <row r="32" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A32" s="24">
+      <c r="A32">
         <v>2019</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32">
         <v>25000</v>
       </c>
     </row>
     <row r="33" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A33" s="24">
+      <c r="A33">
         <v>2019</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="24">
+      <c r="D33">
         <v>23450</v>
       </c>
     </row>
     <row r="34" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A34" s="24">
+      <c r="A34">
         <v>2018</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34">
         <v>32050</v>
       </c>
     </row>
     <row r="35" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A35" s="24">
+      <c r="A35">
         <v>2019</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35">
         <v>31000</v>
       </c>
     </row>
     <row r="36" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A36" s="24">
+      <c r="A36">
         <v>2018</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36">
         <v>31520</v>
       </c>
     </row>
     <row r="37" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A37" s="24">
+      <c r="A37">
         <v>2019</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D37">
         <v>29000</v>
       </c>
     </row>
     <row r="38" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A38" s="24">
+      <c r="A38">
         <v>2018</v>
       </c>
-      <c r="B38" s="24" t="s">
+      <c r="B38" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38">
         <v>30020</v>
       </c>
     </row>
     <row r="39" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A39" s="24">
+      <c r="A39">
         <v>2021</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39">
         <v>44200</v>
       </c>
     </row>
     <row r="40" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A40" s="24">
+      <c r="A40">
         <v>2021</v>
       </c>
-      <c r="B40" s="24" t="s">
+      <c r="B40" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D40">
         <v>24800</v>
       </c>
     </row>
     <row r="41" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A41" s="24">
+      <c r="A41">
         <v>2020</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41">
         <v>22500</v>
       </c>
     </row>
     <row r="42" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A42" s="24">
+      <c r="A42">
         <v>2021</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" t="s">
         <v>26</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42">
         <v>27000</v>
       </c>
     </row>
     <row r="43" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A43" s="24">
+      <c r="A43">
         <v>2021</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="24">
+      <c r="D43">
         <v>31500</v>
       </c>
     </row>
     <row r="44" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A44" s="24">
+      <c r="A44">
         <v>2022</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D44">
         <v>27000</v>
       </c>
     </row>
     <row r="45" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A45" s="24">
+      <c r="A45">
         <v>2019</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45">
         <v>24500</v>
       </c>
     </row>
     <row r="46" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A46" s="24">
+      <c r="A46">
         <v>2019</v>
       </c>
-      <c r="B46" s="24" t="s">
+      <c r="B46" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46">
         <v>24800</v>
       </c>
     </row>
     <row r="47" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B47" s="24">
+      <c r="B47">
         <f>SUBTOTAL(9,B22:B46)</f>
         <v>0</v>
       </c>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24">
+      <c r="D47">
         <f>SUBTOTAL(9,D22:D46)</f>
         <v>708470</v>
       </c>
     </row>
     <row r="48" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A48" s="24">
+      <c r="A48">
         <v>2021</v>
       </c>
-      <c r="B48" s="24" t="s">
+      <c r="B48" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="24">
+      <c r="D48">
         <v>31500</v>
       </c>
     </row>
     <row r="49" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A49" s="24">
+      <c r="A49">
         <v>2018</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B49" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49">
         <v>32050</v>
       </c>
     </row>
     <row r="50" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A50" s="24">
+      <c r="A50">
         <v>2019</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" t="s">
         <v>22</v>
       </c>
-      <c r="D50" s="24">
+      <c r="D50">
         <v>23800</v>
       </c>
     </row>
     <row r="51" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A51" s="24">
+      <c r="A51">
         <v>2020</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="24">
+      <c r="D51">
         <v>19430</v>
       </c>
     </row>
     <row r="52" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A52" s="24">
+      <c r="A52">
         <v>2021</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="24">
+      <c r="D52">
         <v>25300</v>
       </c>
     </row>
     <row r="53" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A53" s="24">
+      <c r="A53">
         <v>2018</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B53" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="24">
+      <c r="D53">
         <v>26500</v>
       </c>
     </row>
     <row r="54" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A54" s="24">
+      <c r="A54">
         <v>2020</v>
       </c>
-      <c r="B54" s="24" t="s">
+      <c r="B54" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" t="s">
         <v>26</v>
       </c>
-      <c r="D54" s="24">
+      <c r="D54">
         <v>26000</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A55" s="24">
+      <c r="A55">
         <v>2020</v>
       </c>
-      <c r="B55" s="24" t="s">
+      <c r="B55" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C55" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="24">
+      <c r="D55">
         <v>22500</v>
       </c>
     </row>
     <row r="56" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A56" s="24">
+      <c r="A56">
         <v>2018</v>
       </c>
-      <c r="B56" s="24" t="s">
+      <c r="B56" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="24" t="s">
+      <c r="C56" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="24">
+      <c r="D56">
         <v>30020</v>
       </c>
     </row>
     <row r="57" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A57" s="24">
+      <c r="A57">
         <v>2021</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B57" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="24" t="s">
+      <c r="C57" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57">
         <v>25000</v>
       </c>
     </row>
     <row r="58" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A58" s="24">
+      <c r="A58">
         <v>2022</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="B58" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="24">
+      <c r="D58">
         <v>27000</v>
       </c>
     </row>
     <row r="59" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A59" s="24">
+      <c r="A59">
         <v>2019</v>
       </c>
-      <c r="B59" s="24" t="s">
+      <c r="B59" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="24">
+      <c r="D59">
         <v>21800</v>
       </c>
     </row>
     <row r="60" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A60" s="24">
+      <c r="A60">
         <v>2020</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B60" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C60" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="24">
+      <c r="D60">
         <v>24500</v>
       </c>
     </row>
     <row r="61" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A61" s="24">
+      <c r="A61">
         <v>2022</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B61" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="24" t="s">
+      <c r="C61" t="s">
         <v>22</v>
       </c>
-      <c r="D61" s="24">
+      <c r="D61">
         <v>25500</v>
       </c>
     </row>
     <row r="62" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A62" s="24">
+      <c r="A62">
         <v>2020</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B62" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="24" t="s">
+      <c r="C62" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="24">
+      <c r="D62">
         <v>19430</v>
       </c>
     </row>
     <row r="63" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A63" s="24">
+      <c r="A63">
         <v>2021</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B63" t="s">
         <v>8</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C63" t="s">
         <v>9</v>
       </c>
-      <c r="D63" s="24">
+      <c r="D63">
         <v>31500</v>
       </c>
     </row>
     <row r="64" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A64" s="24">
+      <c r="A64">
         <v>2020</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" t="s">
         <v>8</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" t="s">
         <v>17</v>
       </c>
-      <c r="D64" s="24">
+      <c r="D64">
         <v>19800</v>
       </c>
     </row>
     <row r="65" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A65" s="24">
+      <c r="A65">
         <v>2020</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B65" t="s">
         <v>8</v>
       </c>
-      <c r="C65" s="24" t="s">
+      <c r="C65" t="s">
         <v>13</v>
       </c>
-      <c r="D65" s="24">
+      <c r="D65">
         <v>29500</v>
       </c>
     </row>
     <row r="66" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="23" t="s">
+      <c r="A66" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B66" s="24">
+      <c r="B66">
         <f>SUBTOTAL(9,B48:B65)</f>
         <v>0</v>
       </c>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24">
+      <c r="D66">
         <f>SUBTOTAL(9,D48:D65)</f>
         <v>461130</v>
       </c>
     </row>
     <row r="67" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A67" s="24">
+      <c r="A67">
         <v>2019</v>
       </c>
-      <c r="B67" s="24" t="s">
+      <c r="B67" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="24" t="s">
+      <c r="C67" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="24">
+      <c r="D67">
         <v>23450</v>
       </c>
     </row>
     <row r="68" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A68" s="24">
+      <c r="A68">
         <v>2021</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B68" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="C68" t="s">
         <v>11</v>
       </c>
-      <c r="D68" s="24">
+      <c r="D68">
         <v>25300</v>
       </c>
     </row>
     <row r="69" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A69" s="24">
+      <c r="A69">
         <v>2020</v>
       </c>
-      <c r="B69" s="24" t="s">
+      <c r="B69" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="24" t="s">
+      <c r="C69" t="s">
         <v>13</v>
       </c>
-      <c r="D69" s="24">
+      <c r="D69">
         <v>29500</v>
       </c>
     </row>
     <row r="70" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A70" s="24">
+      <c r="A70">
         <v>2018</v>
       </c>
-      <c r="B70" s="24" t="s">
+      <c r="B70" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C70" t="s">
         <v>7</v>
       </c>
-      <c r="D70" s="24">
+      <c r="D70">
         <v>30020</v>
       </c>
     </row>
     <row r="71" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A71" s="24">
+      <c r="A71">
         <v>2020</v>
       </c>
-      <c r="B71" s="24" t="s">
+      <c r="B71" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="24" t="s">
+      <c r="C71" t="s">
         <v>17</v>
       </c>
-      <c r="D71" s="24">
+      <c r="D71">
         <v>23000</v>
       </c>
     </row>
     <row r="72" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A72" s="24">
+      <c r="A72">
         <v>2021</v>
       </c>
-      <c r="B72" s="24" t="s">
+      <c r="B72" t="s">
         <v>6</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C72" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="24">
+      <c r="D72">
         <v>24800</v>
       </c>
     </row>
     <row r="73" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A73" s="24">
+      <c r="A73">
         <v>2021</v>
       </c>
-      <c r="B73" s="24" t="s">
+      <c r="B73" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="24" t="s">
+      <c r="C73" t="s">
         <v>9</v>
       </c>
-      <c r="D73" s="24">
+      <c r="D73">
         <v>31500</v>
       </c>
     </row>
     <row r="74" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A74" s="24">
+      <c r="A74">
         <v>2020</v>
       </c>
-      <c r="B74" s="24" t="s">
+      <c r="B74" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="24" t="s">
+      <c r="C74" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="24">
+      <c r="D74">
         <v>19430</v>
       </c>
     </row>
     <row r="75" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A75" s="24">
+      <c r="A75">
         <v>2018</v>
       </c>
-      <c r="B75" s="24" t="s">
+      <c r="B75" t="s">
         <v>6</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" t="s">
         <v>9</v>
       </c>
-      <c r="D75" s="24">
+      <c r="D75">
         <v>26500</v>
       </c>
     </row>
     <row r="76" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A76" s="24">
+      <c r="A76">
         <v>2020</v>
       </c>
-      <c r="B76" s="24" t="s">
+      <c r="B76" t="s">
         <v>6</v>
       </c>
-      <c r="C76" s="24" t="s">
+      <c r="C76" t="s">
         <v>26</v>
       </c>
-      <c r="D76" s="24">
+      <c r="D76">
         <v>26000</v>
       </c>
     </row>
     <row r="77" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A77" s="24">
+      <c r="A77">
         <v>2019</v>
       </c>
-      <c r="B77" s="24" t="s">
+      <c r="B77" t="s">
         <v>6</v>
       </c>
-      <c r="C77" s="24" t="s">
+      <c r="C77" t="s">
         <v>17</v>
       </c>
-      <c r="D77" s="24">
+      <c r="D77">
         <v>21800</v>
       </c>
     </row>
     <row r="78" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A78" s="24">
+      <c r="A78">
         <v>2020</v>
       </c>
-      <c r="B78" s="24" t="s">
+      <c r="B78" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="24" t="s">
+      <c r="C78" t="s">
         <v>17</v>
       </c>
-      <c r="D78" s="24">
+      <c r="D78">
         <v>22500</v>
       </c>
     </row>
     <row r="79" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A79" s="24">
+      <c r="A79">
         <v>2022</v>
       </c>
-      <c r="B79" s="24" t="s">
+      <c r="B79" t="s">
         <v>6</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C79" t="s">
         <v>11</v>
       </c>
-      <c r="D79" s="24">
+      <c r="D79">
         <v>27000</v>
       </c>
     </row>
     <row r="80" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A80" s="24">
+      <c r="A80">
         <v>2019</v>
       </c>
-      <c r="B80" s="24" t="s">
+      <c r="B80" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="24" t="s">
+      <c r="C80" t="s">
         <v>13</v>
       </c>
-      <c r="D80" s="24">
+      <c r="D80">
         <v>29000</v>
       </c>
     </row>
     <row r="81" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A81" s="24">
+      <c r="A81">
         <v>2019</v>
       </c>
-      <c r="B81" s="24" t="s">
+      <c r="B81" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="24" t="s">
+      <c r="C81" t="s">
         <v>19</v>
       </c>
-      <c r="D81" s="24">
+      <c r="D81">
         <v>33000</v>
       </c>
     </row>
     <row r="82" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A82" s="24">
+      <c r="A82">
         <v>2022</v>
       </c>
-      <c r="B82" s="24" t="s">
+      <c r="B82" t="s">
         <v>6</v>
       </c>
-      <c r="C82" s="24" t="s">
+      <c r="C82" t="s">
         <v>22</v>
       </c>
-      <c r="D82" s="24">
+      <c r="D82">
         <v>25500</v>
       </c>
     </row>
     <row r="83" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A83" s="24">
+      <c r="A83">
         <v>2019</v>
       </c>
-      <c r="B83" s="24" t="s">
+      <c r="B83" t="s">
         <v>6</v>
       </c>
-      <c r="C83" s="24" t="s">
+      <c r="C83" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="24">
+      <c r="D83">
         <v>31000</v>
       </c>
     </row>
     <row r="84" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A84" s="24">
+      <c r="A84">
         <v>2019</v>
       </c>
-      <c r="B84" s="24" t="s">
+      <c r="B84" t="s">
         <v>6</v>
       </c>
-      <c r="C84" s="24" t="s">
+      <c r="C84" t="s">
         <v>20</v>
       </c>
-      <c r="D84" s="24">
+      <c r="D84">
         <v>23450</v>
       </c>
     </row>
     <row r="85" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A85" s="24">
+      <c r="A85">
         <v>2020</v>
       </c>
-      <c r="B85" s="24" t="s">
+      <c r="B85" t="s">
         <v>6</v>
       </c>
-      <c r="C85" s="24" t="s">
+      <c r="C85" t="s">
         <v>11</v>
       </c>
-      <c r="D85" s="24">
+      <c r="D85">
         <v>24500</v>
       </c>
     </row>
     <row r="86" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A86" s="24">
+      <c r="A86">
         <v>2022</v>
       </c>
-      <c r="B86" s="24" t="s">
+      <c r="B86" t="s">
         <v>6</v>
       </c>
-      <c r="C86" s="24" t="s">
+      <c r="C86" t="s">
         <v>13</v>
       </c>
-      <c r="D86" s="24">
+      <c r="D86">
         <v>53000</v>
       </c>
     </row>
     <row r="87" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A87" s="24">
+      <c r="A87">
         <v>2021</v>
       </c>
-      <c r="B87" s="24" t="s">
+      <c r="B87" t="s">
         <v>6</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" t="s">
         <v>26</v>
       </c>
-      <c r="D87" s="24">
+      <c r="D87">
         <v>27000</v>
       </c>
     </row>
     <row r="88" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A88" s="24">
+      <c r="A88">
         <v>2021</v>
       </c>
-      <c r="B88" s="24" t="s">
+      <c r="B88" t="s">
         <v>6</v>
       </c>
-      <c r="C88" s="24" t="s">
+      <c r="C88" t="s">
         <v>20</v>
       </c>
-      <c r="D88" s="24">
+      <c r="D88">
         <v>44200</v>
       </c>
     </row>
     <row r="89" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A89" s="24">
+      <c r="A89">
         <v>2018</v>
       </c>
-      <c r="B89" s="24" t="s">
+      <c r="B89" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="24" t="s">
+      <c r="C89" t="s">
         <v>15</v>
       </c>
-      <c r="D89" s="24">
+      <c r="D89">
         <v>31520</v>
       </c>
     </row>
     <row r="90" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A90" s="24">
+      <c r="A90">
         <v>2021</v>
       </c>
-      <c r="B90" s="24" t="s">
+      <c r="B90" t="s">
         <v>6</v>
       </c>
-      <c r="C90" s="24" t="s">
+      <c r="C90" t="s">
         <v>7</v>
       </c>
-      <c r="D90" s="24">
+      <c r="D90">
         <v>29450</v>
       </c>
     </row>
     <row r="91" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A91" s="24">
+      <c r="A91">
         <v>2022</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B91" t="s">
         <v>6</v>
       </c>
-      <c r="C91" s="24" t="s">
+      <c r="C91" t="s">
         <v>22</v>
       </c>
-      <c r="D91" s="24">
+      <c r="D91">
         <v>25500</v>
       </c>
     </row>
     <row r="92" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A92" s="24">
+      <c r="A92">
         <v>2021</v>
       </c>
-      <c r="B92" s="24" t="s">
+      <c r="B92" t="s">
         <v>6</v>
       </c>
-      <c r="C92" s="24" t="s">
+      <c r="C92" t="s">
         <v>5</v>
       </c>
-      <c r="D92" s="24">
+      <c r="D92">
         <v>25000</v>
       </c>
     </row>
     <row r="93" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A93" s="24">
+      <c r="A93">
         <v>2020</v>
       </c>
-      <c r="B93" s="24" t="s">
+      <c r="B93" t="s">
         <v>6</v>
       </c>
-      <c r="C93" s="24" t="s">
+      <c r="C93" t="s">
         <v>9</v>
       </c>
-      <c r="D93" s="24">
+      <c r="D93">
         <v>28000</v>
       </c>
     </row>
     <row r="94" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A94" s="24">
+      <c r="A94">
         <v>2021</v>
       </c>
-      <c r="B94" s="24" t="s">
+      <c r="B94" t="s">
         <v>6</v>
       </c>
-      <c r="C94" s="24" t="s">
+      <c r="C94" t="s">
         <v>11</v>
       </c>
-      <c r="D94" s="24">
+      <c r="D94">
         <v>25300</v>
       </c>
     </row>
     <row r="95" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A95" s="24">
+      <c r="A95">
         <v>2018</v>
       </c>
-      <c r="B95" s="24" t="s">
+      <c r="B95" t="s">
         <v>6</v>
       </c>
-      <c r="C95" s="24" t="s">
+      <c r="C95" t="s">
         <v>19</v>
       </c>
-      <c r="D95" s="24">
+      <c r="D95">
         <v>32050</v>
       </c>
     </row>
     <row r="96" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A96" s="24">
+      <c r="A96">
         <v>2019</v>
       </c>
-      <c r="B96" s="24" t="s">
+      <c r="B96" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="24" t="s">
+      <c r="C96" t="s">
         <v>17</v>
       </c>
-      <c r="D96" s="24">
+      <c r="D96">
         <v>21800</v>
       </c>
     </row>
     <row r="97" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A97" s="24">
+      <c r="A97">
         <v>2019</v>
       </c>
-      <c r="B97" s="24" t="s">
+      <c r="B97" t="s">
         <v>6</v>
       </c>
-      <c r="C97" s="24" t="s">
+      <c r="C97" t="s">
         <v>13</v>
       </c>
-      <c r="D97" s="24">
+      <c r="D97">
         <v>29000</v>
       </c>
     </row>
     <row r="98" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A98" s="24">
+      <c r="A98">
         <v>2021</v>
       </c>
-      <c r="B98" s="24" t="s">
+      <c r="B98" t="s">
         <v>6</v>
       </c>
-      <c r="C98" s="24" t="s">
+      <c r="C98" t="s">
         <v>5</v>
       </c>
-      <c r="D98" s="24">
+      <c r="D98">
         <v>25000</v>
       </c>
     </row>
     <row r="99" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A99" s="24">
+      <c r="A99">
         <v>2022</v>
       </c>
-      <c r="B99" s="24" t="s">
+      <c r="B99" t="s">
         <v>6</v>
       </c>
-      <c r="C99" s="24" t="s">
+      <c r="C99" t="s">
         <v>13</v>
       </c>
-      <c r="D99" s="24">
+      <c r="D99">
         <v>52300</v>
       </c>
     </row>
     <row r="100" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="23" t="s">
+      <c r="A100" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B100" s="24">
+      <c r="B100">
         <f>SUBTOTAL(9,B67:B99)</f>
         <v>0</v>
       </c>
-      <c r="C100" s="24"/>
-      <c r="D100" s="24">
+      <c r="D100">
         <f>SUBTOTAL(9,D67:D99)</f>
         <v>946370</v>
       </c>
     </row>
     <row r="101" spans="1:4" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A101" s="24">
+      <c r="A101">
         <v>2019</v>
       </c>
-      <c r="B101" s="24" t="s">
+      <c r="B101" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="24" t="s">
+      <c r="C101" t="s">
         <v>24</v>
       </c>
-      <c r="D101" s="24">
+      <c r="D101">
         <v>24800</v>
       </c>
     </row>
     <row r="102" spans="1:4" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="23" t="s">
+      <c r="A102" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B102" s="24">
+      <c r="B102">
         <f>SUBTOTAL(9,B101:B101)</f>
         <v>0</v>
       </c>
-      <c r="C102" s="24"/>
-      <c r="D102" s="24">
+      <c r="D102">
         <f>SUBTOTAL(9,D101:D101)</f>
         <v>24800</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="23" t="s">
+      <c r="A103" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B103" s="24">
+      <c r="B103">
         <f>SUBTOTAL(9,B2:B101)</f>
         <v>0</v>
       </c>
-      <c r="C103" s="24"/>
-      <c r="D103" s="24">
+      <c r="D103">
         <f>SUBTOTAL(9,D2:D101)</f>
         <v>2660440</v>
       </c>

</xml_diff>